<commit_message>
Edited .gitignore and test files
</commit_message>
<xml_diff>
--- a/S Roster and Attendance - Spring 2025.xlsx
+++ b/S Roster and Attendance - Spring 2025.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="11_3E62A14F91AA8DF2FB2927049584F9E77AABD855" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE60F7A7-B183-4DF0-A679-DA3F5CE3E1B5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8430" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="1" r:id="rId1"/>
@@ -1336,6 +1336,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1543,7 +1547,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>